<commit_message>
final version to test
</commit_message>
<xml_diff>
--- a/Tablas/plantillaRecaudadora.xlsx
+++ b/Tablas/plantillaRecaudadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\Tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939A6AAE-68B1-422F-A09D-B50D7D3AE98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABA1098-F9EB-4D65-87C1-FDCC57CD5671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="750" windowWidth="20265" windowHeight="10770" tabRatio="381" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="381" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PT Distribuidora" sheetId="1" r:id="rId1"/>
@@ -1453,19 +1453,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1484,20 +1471,33 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1810,8 +1810,9 @@
   </sheetPr>
   <dimension ref="A2:CE886"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1937,161 +1938,161 @@
       <c r="H3" s="74"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="M3" s="117" t="s">
+      <c r="M3" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="118"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111"/>
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="111"/>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="112"/>
       <c r="AA3" s="12"/>
       <c r="AB3" s="11"/>
-      <c r="AC3" s="123" t="s">
+      <c r="AC3" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="AD3" s="106"/>
-      <c r="AE3" s="106"/>
-      <c r="AF3" s="106"/>
-      <c r="AG3" s="106"/>
-      <c r="AH3" s="106"/>
-      <c r="AI3" s="106"/>
-      <c r="AJ3" s="106"/>
-      <c r="AK3" s="106"/>
-      <c r="AL3" s="106"/>
-      <c r="AM3" s="106"/>
-      <c r="AN3" s="106"/>
-      <c r="AO3" s="120"/>
-      <c r="AP3" s="122" t="s">
+      <c r="AD3" s="117"/>
+      <c r="AE3" s="117"/>
+      <c r="AF3" s="117"/>
+      <c r="AG3" s="117"/>
+      <c r="AH3" s="117"/>
+      <c r="AI3" s="117"/>
+      <c r="AJ3" s="117"/>
+      <c r="AK3" s="117"/>
+      <c r="AL3" s="117"/>
+      <c r="AM3" s="117"/>
+      <c r="AN3" s="117"/>
+      <c r="AO3" s="114"/>
+      <c r="AP3" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="AQ3" s="106"/>
-      <c r="AR3" s="106"/>
-      <c r="AS3" s="106"/>
-      <c r="AT3" s="106"/>
-      <c r="AU3" s="106"/>
-      <c r="AV3" s="106"/>
-      <c r="AW3" s="120"/>
-      <c r="AX3" s="114" t="s">
+      <c r="AQ3" s="117"/>
+      <c r="AR3" s="117"/>
+      <c r="AS3" s="117"/>
+      <c r="AT3" s="117"/>
+      <c r="AU3" s="117"/>
+      <c r="AV3" s="117"/>
+      <c r="AW3" s="114"/>
+      <c r="AX3" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="AY3" s="115"/>
-      <c r="AZ3" s="115"/>
-      <c r="BA3" s="115"/>
-      <c r="BB3" s="115"/>
-      <c r="BC3" s="115"/>
-      <c r="BD3" s="115"/>
-      <c r="BE3" s="115"/>
-      <c r="BF3" s="115"/>
-      <c r="BG3" s="115"/>
-      <c r="BH3" s="115"/>
-      <c r="BI3" s="115"/>
-      <c r="BJ3" s="115"/>
-      <c r="BK3" s="115"/>
-      <c r="BL3" s="115"/>
-      <c r="BM3" s="115"/>
-      <c r="BN3" s="115"/>
-      <c r="BO3" s="115"/>
-      <c r="BP3" s="116"/>
+      <c r="AY3" s="108"/>
+      <c r="AZ3" s="108"/>
+      <c r="BA3" s="108"/>
+      <c r="BB3" s="108"/>
+      <c r="BC3" s="108"/>
+      <c r="BD3" s="108"/>
+      <c r="BE3" s="108"/>
+      <c r="BF3" s="108"/>
+      <c r="BG3" s="108"/>
+      <c r="BH3" s="108"/>
+      <c r="BI3" s="108"/>
+      <c r="BJ3" s="108"/>
+      <c r="BK3" s="108"/>
+      <c r="BL3" s="108"/>
+      <c r="BM3" s="108"/>
+      <c r="BN3" s="108"/>
+      <c r="BO3" s="108"/>
+      <c r="BP3" s="109"/>
       <c r="BT3" s="6"/>
       <c r="BW3" s="16"/>
       <c r="BX3" s="16"/>
       <c r="BY3" s="34"/>
     </row>
     <row r="4" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="107"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="121"/>
       <c r="H4" s="74"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="111" t="s">
+      <c r="K4" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="110"/>
-      <c r="M4" s="108" t="s">
+      <c r="L4" s="111"/>
+      <c r="M4" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="109"/>
-      <c r="O4" s="108" t="s">
+      <c r="N4" s="123"/>
+      <c r="O4" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="109"/>
-      <c r="Q4" s="108" t="s">
+      <c r="P4" s="123"/>
+      <c r="Q4" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="110"/>
-      <c r="S4" s="109"/>
-      <c r="T4" s="108" t="s">
+      <c r="R4" s="111"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="110"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="111" t="s">
+      <c r="U4" s="111"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="110"/>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="119" t="s">
+      <c r="X4" s="111"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="120"/>
-      <c r="AC4" s="123" t="s">
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="106"/>
-      <c r="AE4" s="120"/>
-      <c r="AF4" s="123" t="s">
+      <c r="AD4" s="117"/>
+      <c r="AE4" s="114"/>
+      <c r="AF4" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="AG4" s="106"/>
-      <c r="AH4" s="120"/>
-      <c r="AI4" s="123" t="s">
+      <c r="AG4" s="117"/>
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="AJ4" s="106"/>
-      <c r="AK4" s="106"/>
-      <c r="AL4" s="106"/>
-      <c r="AM4" s="120"/>
-      <c r="AN4" s="123" t="s">
+      <c r="AJ4" s="117"/>
+      <c r="AK4" s="117"/>
+      <c r="AL4" s="117"/>
+      <c r="AM4" s="114"/>
+      <c r="AN4" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="AO4" s="120"/>
-      <c r="AP4" s="121" t="s">
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="AQ4" s="106"/>
-      <c r="AR4" s="106"/>
-      <c r="AS4" s="120"/>
-      <c r="AT4" s="122" t="s">
+      <c r="AQ4" s="117"/>
+      <c r="AR4" s="117"/>
+      <c r="AS4" s="114"/>
+      <c r="AT4" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="AU4" s="106"/>
-      <c r="AV4" s="106"/>
-      <c r="AW4" s="120"/>
+      <c r="AU4" s="117"/>
+      <c r="AV4" s="117"/>
+      <c r="AW4" s="114"/>
       <c r="AX4" s="99"/>
       <c r="AY4" s="98"/>
       <c r="AZ4" s="100"/>
       <c r="BA4" s="97"/>
-      <c r="BB4" s="112" t="s">
+      <c r="BB4" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="BC4" s="113"/>
+      <c r="BC4" s="106"/>
       <c r="BD4" s="102" t="s">
         <v>16</v>
       </c>
@@ -77225,6 +77226,12 @@
   </sheetData>
   <autoFilter ref="A6:BI6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="19">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="AX3:BP3"/>
     <mergeCell ref="M3:Z3"/>
@@ -77238,12 +77245,6 @@
     <mergeCell ref="AC3:AO3"/>
     <mergeCell ref="AN4:AO4"/>
     <mergeCell ref="AP3:AW3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="Q4:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -77255,7 +77256,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -77291,50 +77295,50 @@
       <c r="I5" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="106"/>
-      <c r="K5" s="120"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="114"/>
       <c r="L5" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="M5" s="106"/>
-      <c r="N5" s="120"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="114"/>
       <c r="O5" s="127" t="s">
         <v>67</v>
       </c>
       <c r="S5" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="T5" s="120"/>
+      <c r="T5" s="114"/>
       <c r="U5" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="120"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="117"/>
+      <c r="X5" s="114"/>
       <c r="Y5" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="120"/>
+      <c r="Z5" s="117"/>
+      <c r="AA5" s="114"/>
       <c r="AB5" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="AC5" s="106"/>
-      <c r="AD5" s="106"/>
-      <c r="AE5" s="120"/>
+      <c r="AC5" s="117"/>
+      <c r="AD5" s="117"/>
+      <c r="AE5" s="114"/>
       <c r="AF5" s="130" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" s="106"/>
-      <c r="AH5" s="106"/>
-      <c r="AI5" s="106"/>
-      <c r="AJ5" s="120"/>
+      <c r="AG5" s="117"/>
+      <c r="AH5" s="117"/>
+      <c r="AI5" s="117"/>
+      <c r="AJ5" s="114"/>
       <c r="AK5" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="AL5" s="106"/>
-      <c r="AM5" s="106"/>
-      <c r="AN5" s="120"/>
+      <c r="AL5" s="117"/>
+      <c r="AM5" s="117"/>
+      <c r="AN5" s="114"/>
     </row>
     <row r="6" spans="1:41" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">

</xml_diff>